<commit_message>
Conversão de variáveis, *, NaN para .
</commit_message>
<xml_diff>
--- a/rotulos_colunas/rotulos_colunas_todas_bases.xlsx
+++ b/rotulos_colunas/rotulos_colunas_todas_bases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/Meu Drive/Doutorado/Disciplinas/Estatística/Projeto/projeto-enade-estatistica-1/rotulos_colunas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42347C53-AF19-1744-88D3-8B7F4C6563CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB579459-580D-9F49-ABF2-B4EFF187A574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="1920" windowWidth="35500" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1985,10 +1985,10 @@
   <dimension ref="A1:K228"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B217" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J72" sqref="J72"/>
+      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Bases de dados filtradas
</commit_message>
<xml_diff>
--- a/rotulos_colunas/rotulos_colunas_todas_bases.xlsx
+++ b/rotulos_colunas/rotulos_colunas_todas_bases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/Meu Drive/Doutorado/Disciplinas/Estatística/Projeto/projeto-enade-estatistica-1/rotulos_colunas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB579459-580D-9F49-ABF2-B4EFF187A574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A223512-85E2-3043-AFCE-26188AB3D4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="1920" windowWidth="35500" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1985,10 +1985,10 @@
   <dimension ref="A1:K228"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B217" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>